<commit_message>
perfect sample_metadata for skq21_12S
</commit_message>
<xml_diff>
--- a/dy2012/faire_mapping_and_output/sample_metadata_files/dy2012_faire_metadata.xlsx
+++ b/dy2012/faire_mapping_and_output/sample_metadata_files/dy2012_faire_metadata.xlsx
@@ -7757,11 +7757,11 @@
         </is>
       </c>
       <c r="J4" t="n">
+        <v>-171.69841</v>
+      </c>
+      <c r="K4" t="n">
         <v>59.904865</v>
       </c>
-      <c r="K4" t="n">
-        <v>-171.69841</v>
-      </c>
       <c r="L4" t="inlineStr">
         <is>
           <t>171˚ 41.905' W</t>
@@ -7834,7 +7834,7 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA4" t="n">
@@ -8411,15 +8411,15 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>E26.1B.DY2012 | E26.2B.DY2012</t>
+          <t>E26.2B.DY2012 | E26.1B.DY2012</t>
         </is>
       </c>
       <c r="J5" t="n">
+        <v>-171.69841</v>
+      </c>
+      <c r="K5" t="n">
         <v>59.904865</v>
       </c>
-      <c r="K5" t="n">
-        <v>-171.69841</v>
-      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>171˚ 41.905' W</t>
@@ -8492,7 +8492,7 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA5" t="n">
@@ -9069,15 +9069,15 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>E26.1B.DY2012 | E26.2B.DY2012</t>
+          <t>E26.2B.DY2012 | E26.1B.DY2012</t>
         </is>
       </c>
       <c r="J6" t="n">
+        <v>-171.69841</v>
+      </c>
+      <c r="K6" t="n">
         <v>59.904865</v>
       </c>
-      <c r="K6" t="n">
-        <v>-171.69841</v>
-      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>171˚ 41.905' W</t>
@@ -9150,7 +9150,7 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA6" t="n">
@@ -9731,11 +9731,11 @@
         </is>
       </c>
       <c r="J7" t="n">
+        <v>-174.0845</v>
+      </c>
+      <c r="K7" t="n">
         <v>62.4666</v>
       </c>
-      <c r="K7" t="n">
-        <v>-174.0845</v>
-      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>174˚ 05.070' W</t>
@@ -9808,7 +9808,7 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA7" t="n">
@@ -10389,11 +10389,11 @@
         </is>
       </c>
       <c r="J8" t="n">
+        <v>-174.0845</v>
+      </c>
+      <c r="K8" t="n">
         <v>62.4666</v>
       </c>
-      <c r="K8" t="n">
-        <v>-174.0845</v>
-      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>174˚ 05.070' W</t>
@@ -10466,7 +10466,7 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA8" t="n">
@@ -11043,15 +11043,15 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>E28.1B.DY2012 | E28.2B.DY2012</t>
+          <t>E28.2B.DY2012 | E28.1B.DY2012</t>
         </is>
       </c>
       <c r="J9" t="n">
+        <v>-174.0845</v>
+      </c>
+      <c r="K9" t="n">
         <v>62.4666</v>
       </c>
-      <c r="K9" t="n">
-        <v>-174.0845</v>
-      </c>
       <c r="L9" t="inlineStr">
         <is>
           <t>174˚ 05.070' W</t>
@@ -11124,7 +11124,7 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA9" t="n">
@@ -11701,15 +11701,15 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>E28.1B.DY2012 | E28.2B.DY2012</t>
+          <t>E28.2B.DY2012 | E28.1B.DY2012</t>
         </is>
       </c>
       <c r="J10" t="n">
+        <v>-174.0845</v>
+      </c>
+      <c r="K10" t="n">
         <v>62.4666</v>
       </c>
-      <c r="K10" t="n">
-        <v>-174.0845</v>
-      </c>
       <c r="L10" t="inlineStr">
         <is>
           <t>174˚ 05.070' W</t>
@@ -11782,7 +11782,7 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA10" t="n">
@@ -12359,15 +12359,15 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>E29.1B.DY2012 | E29.2B.DY2012</t>
+          <t>E29.2B.DY2012 | E29.1B.DY2012</t>
         </is>
       </c>
       <c r="J11" t="n">
+        <v>-175.06967</v>
+      </c>
+      <c r="K11" t="n">
         <v>62.010666</v>
       </c>
-      <c r="K11" t="n">
-        <v>-175.06967</v>
-      </c>
       <c r="L11" t="inlineStr">
         <is>
           <t>175˚ 04.18' W</t>
@@ -12440,7 +12440,7 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA11" t="n">
@@ -13017,15 +13017,15 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>E29.1B.DY2012 | E29.2B.DY2012</t>
+          <t>E29.2B.DY2012 | E29.1B.DY2012</t>
         </is>
       </c>
       <c r="J12" t="n">
+        <v>-175.06967</v>
+      </c>
+      <c r="K12" t="n">
         <v>62.010666</v>
       </c>
-      <c r="K12" t="n">
-        <v>-175.06967</v>
-      </c>
       <c r="L12" t="inlineStr">
         <is>
           <t>175˚ 04.18' W</t>
@@ -13098,7 +13098,7 @@
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA12" t="n">
@@ -13675,15 +13675,15 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>E30.2B.DY2012 | E30.1B.DY2012</t>
+          <t>E30.1B.DY2012 | E30.2B.DY2012</t>
         </is>
       </c>
       <c r="J13" t="n">
+        <v>-175.06967</v>
+      </c>
+      <c r="K13" t="n">
         <v>62.010666</v>
       </c>
-      <c r="K13" t="n">
-        <v>-175.06967</v>
-      </c>
       <c r="L13" t="inlineStr">
         <is>
           <t>175˚ 04.18' W</t>
@@ -13756,7 +13756,7 @@
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA13" t="n">
@@ -14333,15 +14333,15 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>E30.2B.DY2012 | E30.1B.DY2012</t>
+          <t>E30.1B.DY2012 | E30.2B.DY2012</t>
         </is>
       </c>
       <c r="J14" t="n">
+        <v>-175.06967</v>
+      </c>
+      <c r="K14" t="n">
         <v>62.010666</v>
       </c>
-      <c r="K14" t="n">
-        <v>-175.06967</v>
-      </c>
       <c r="L14" t="inlineStr">
         <is>
           <t>175˚ 04.18' W</t>
@@ -14414,7 +14414,7 @@
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA14" t="n">
@@ -14991,15 +14991,15 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>E31.1B.DY2012 | E31.2B.DY2012</t>
+          <t>E31.2B.DY2012 | E31.1B.DY2012</t>
         </is>
       </c>
       <c r="J15" t="n">
+        <v>-174.87817</v>
+      </c>
+      <c r="K15" t="n">
         <v>62.217834</v>
       </c>
-      <c r="K15" t="n">
-        <v>-174.87817</v>
-      </c>
       <c r="L15" t="inlineStr">
         <is>
           <t>174˚ 52.69' W</t>
@@ -15072,7 +15072,7 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA15" t="n">
@@ -15649,15 +15649,15 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>E31.1B.DY2012 | E31.2B.DY2012</t>
+          <t>E31.2B.DY2012 | E31.1B.DY2012</t>
         </is>
       </c>
       <c r="J16" t="n">
+        <v>-174.87817</v>
+      </c>
+      <c r="K16" t="n">
         <v>62.217834</v>
       </c>
-      <c r="K16" t="n">
-        <v>-174.87817</v>
-      </c>
       <c r="L16" t="inlineStr">
         <is>
           <t>174˚ 52.69' W</t>
@@ -15730,7 +15730,7 @@
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA16" t="n">
@@ -16311,11 +16311,11 @@
         </is>
       </c>
       <c r="J17" t="n">
+        <v>-174.87817</v>
+      </c>
+      <c r="K17" t="n">
         <v>62.217834</v>
       </c>
-      <c r="K17" t="n">
-        <v>-174.87817</v>
-      </c>
       <c r="L17" t="inlineStr">
         <is>
           <t>174˚ 52.69' W</t>
@@ -16388,7 +16388,7 @@
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA17" t="n">
@@ -16969,11 +16969,11 @@
         </is>
       </c>
       <c r="J18" t="n">
+        <v>-174.87817</v>
+      </c>
+      <c r="K18" t="n">
         <v>62.217834</v>
       </c>
-      <c r="K18" t="n">
-        <v>-174.87817</v>
-      </c>
       <c r="L18" t="inlineStr">
         <is>
           <t>174˚ 52.69' W</t>
@@ -17046,7 +17046,7 @@
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA18" t="n">
@@ -17623,15 +17623,15 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>E33.1B.DY2012 | E33.2B.DY2012</t>
+          <t>E33.2B.DY2012 | E33.1B.DY2012</t>
         </is>
       </c>
       <c r="J19" t="n">
+        <v>-174.69914</v>
+      </c>
+      <c r="K19" t="n">
         <v>62.20373</v>
       </c>
-      <c r="K19" t="n">
-        <v>-174.69914</v>
-      </c>
       <c r="L19" t="inlineStr">
         <is>
           <t>174˚ 41.949' W</t>
@@ -17704,7 +17704,7 @@
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA19" t="n">
@@ -18281,15 +18281,15 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>E33.1B.DY2012 | E33.2B.DY2012</t>
+          <t>E33.2B.DY2012 | E33.1B.DY2012</t>
         </is>
       </c>
       <c r="J20" t="n">
+        <v>-174.69914</v>
+      </c>
+      <c r="K20" t="n">
         <v>62.20373</v>
       </c>
-      <c r="K20" t="n">
-        <v>-174.69914</v>
-      </c>
       <c r="L20" t="inlineStr">
         <is>
           <t>174˚ 41.949' W</t>
@@ -18362,7 +18362,7 @@
       </c>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA20" t="n">
@@ -18939,15 +18939,15 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>E34.1B.DY2012 | E34.2B.DY2012</t>
+          <t>E34.2B.DY2012 | E34.1B.DY2012</t>
         </is>
       </c>
       <c r="J21" t="n">
+        <v>-174.69914</v>
+      </c>
+      <c r="K21" t="n">
         <v>62.20373</v>
       </c>
-      <c r="K21" t="n">
-        <v>-174.69914</v>
-      </c>
       <c r="L21" t="inlineStr">
         <is>
           <t>174˚ 41.949' W</t>
@@ -19020,7 +19020,7 @@
       </c>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA21" t="n">
@@ -19597,15 +19597,15 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>E34.1B.DY2012 | E34.2B.DY2012</t>
+          <t>E34.2B.DY2012 | E34.1B.DY2012</t>
         </is>
       </c>
       <c r="J22" t="n">
+        <v>-174.69914</v>
+      </c>
+      <c r="K22" t="n">
         <v>62.20373</v>
       </c>
-      <c r="K22" t="n">
-        <v>-174.69914</v>
-      </c>
       <c r="L22" t="inlineStr">
         <is>
           <t>174˚ 41.949' W</t>
@@ -19678,7 +19678,7 @@
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA22" t="n">
@@ -20259,11 +20259,11 @@
         </is>
       </c>
       <c r="J23" t="n">
+        <v>-173.4975</v>
+      </c>
+      <c r="K23" t="n">
         <v>62.789684</v>
       </c>
-      <c r="K23" t="n">
-        <v>-173.4975</v>
-      </c>
       <c r="L23" t="inlineStr">
         <is>
           <t>173˚ 29.850' W</t>
@@ -20336,7 +20336,7 @@
       </c>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA23" t="n">
@@ -20917,11 +20917,11 @@
         </is>
       </c>
       <c r="J24" t="n">
+        <v>-173.4975</v>
+      </c>
+      <c r="K24" t="n">
         <v>62.789684</v>
       </c>
-      <c r="K24" t="n">
-        <v>-173.4975</v>
-      </c>
       <c r="L24" t="inlineStr">
         <is>
           <t>173˚ 29.850' W</t>
@@ -20994,7 +20994,7 @@
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA24" t="n">
@@ -21571,15 +21571,15 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>E36.1B.DY2012 | E36.2B.DY2012</t>
+          <t>E36.2B.DY2012 | E36.1B.DY2012</t>
         </is>
       </c>
       <c r="J25" t="n">
+        <v>-173.4975</v>
+      </c>
+      <c r="K25" t="n">
         <v>62.789684</v>
       </c>
-      <c r="K25" t="n">
-        <v>-173.4975</v>
-      </c>
       <c r="L25" t="inlineStr">
         <is>
           <t>173˚ 29.850' W</t>
@@ -21652,7 +21652,7 @@
       </c>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA25" t="n">
@@ -22229,15 +22229,15 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>E36.1B.DY2012 | E36.2B.DY2012</t>
+          <t>E36.2B.DY2012 | E36.1B.DY2012</t>
         </is>
       </c>
       <c r="J26" t="n">
+        <v>-173.4975</v>
+      </c>
+      <c r="K26" t="n">
         <v>62.789684</v>
       </c>
-      <c r="K26" t="n">
-        <v>-173.4975</v>
-      </c>
       <c r="L26" t="inlineStr">
         <is>
           <t>173˚ 29.850' W</t>
@@ -22310,7 +22310,7 @@
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA26" t="n">
@@ -22887,15 +22887,15 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>E37.2B.DY2012 | E37.1B.DY2012</t>
+          <t>E37.1B.DY2012 | E37.2B.DY2012</t>
         </is>
       </c>
       <c r="J27" t="n">
+        <v>-173.28798</v>
+      </c>
+      <c r="K27" t="n">
         <v>63.275066</v>
       </c>
-      <c r="K27" t="n">
-        <v>-173.28798</v>
-      </c>
       <c r="L27" t="inlineStr">
         <is>
           <t>173˚ 17.279' W</t>
@@ -22968,7 +22968,7 @@
       </c>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA27" t="n">
@@ -23545,15 +23545,15 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>E37.2B.DY2012 | E37.1B.DY2012</t>
+          <t>E37.1B.DY2012 | E37.2B.DY2012</t>
         </is>
       </c>
       <c r="J28" t="n">
+        <v>-173.28798</v>
+      </c>
+      <c r="K28" t="n">
         <v>63.275066</v>
       </c>
-      <c r="K28" t="n">
-        <v>-173.28798</v>
-      </c>
       <c r="L28" t="inlineStr">
         <is>
           <t>173˚ 17.279' W</t>
@@ -23626,7 +23626,7 @@
       </c>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA28" t="n">
@@ -24207,11 +24207,11 @@
         </is>
       </c>
       <c r="J29" t="n">
+        <v>-173.28798</v>
+      </c>
+      <c r="K29" t="n">
         <v>63.275066</v>
       </c>
-      <c r="K29" t="n">
-        <v>-173.28798</v>
-      </c>
       <c r="L29" t="inlineStr">
         <is>
           <t>173˚ 17.279' W</t>
@@ -24284,7 +24284,7 @@
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA29" t="n">
@@ -24865,11 +24865,11 @@
         </is>
       </c>
       <c r="J30" t="n">
+        <v>-173.28798</v>
+      </c>
+      <c r="K30" t="n">
         <v>63.275066</v>
       </c>
-      <c r="K30" t="n">
-        <v>-173.28798</v>
-      </c>
       <c r="L30" t="inlineStr">
         <is>
           <t>173˚ 17.279' W</t>
@@ -24942,7 +24942,7 @@
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA30" t="n">
@@ -25523,11 +25523,11 @@
         </is>
       </c>
       <c r="J31" t="n">
+        <v>-169.92117</v>
+      </c>
+      <c r="K31" t="n">
         <v>64.67441599999999</v>
       </c>
-      <c r="K31" t="n">
-        <v>-169.92117</v>
-      </c>
       <c r="L31" t="inlineStr">
         <is>
           <t>169˚ 55.270' W</t>
@@ -25600,7 +25600,7 @@
       </c>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA31" t="n">
@@ -26181,11 +26181,11 @@
         </is>
       </c>
       <c r="J32" t="n">
+        <v>-169.92117</v>
+      </c>
+      <c r="K32" t="n">
         <v>64.67441599999999</v>
       </c>
-      <c r="K32" t="n">
-        <v>-169.92117</v>
-      </c>
       <c r="L32" t="inlineStr">
         <is>
           <t>169˚ 55.270' W</t>
@@ -26258,7 +26258,7 @@
       </c>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA32" t="n">
@@ -26835,15 +26835,15 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>E40.2B.DY2012 | E40.1B.DY2012</t>
+          <t>E40.1B.DY2012 | E40.2B.DY2012</t>
         </is>
       </c>
       <c r="J33" t="n">
+        <v>-169.92117</v>
+      </c>
+      <c r="K33" t="n">
         <v>64.67441599999999</v>
       </c>
-      <c r="K33" t="n">
-        <v>-169.92117</v>
-      </c>
       <c r="L33" t="inlineStr">
         <is>
           <t>169˚ 55.270' W</t>
@@ -26916,7 +26916,7 @@
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA33" t="n">
@@ -27493,15 +27493,15 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>E40.2B.DY2012 | E40.1B.DY2012</t>
+          <t>E40.1B.DY2012 | E40.2B.DY2012</t>
         </is>
       </c>
       <c r="J34" t="n">
+        <v>-169.92117</v>
+      </c>
+      <c r="K34" t="n">
         <v>64.67441599999999</v>
       </c>
-      <c r="K34" t="n">
-        <v>-169.92117</v>
-      </c>
       <c r="L34" t="inlineStr">
         <is>
           <t>169˚ 55.270' W</t>
@@ -27574,7 +27574,7 @@
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA34" t="n">
@@ -28155,11 +28155,11 @@
         </is>
       </c>
       <c r="J35" t="n">
+        <v>-168.23567</v>
+      </c>
+      <c r="K35" t="n">
         <v>64.66849999999999</v>
       </c>
-      <c r="K35" t="n">
-        <v>-168.23567</v>
-      </c>
       <c r="L35" t="inlineStr">
         <is>
           <t>168˚ 14.14' W</t>
@@ -28232,7 +28232,7 @@
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA35" t="n">
@@ -28813,11 +28813,11 @@
         </is>
       </c>
       <c r="J36" t="n">
+        <v>-168.23567</v>
+      </c>
+      <c r="K36" t="n">
         <v>64.66849999999999</v>
       </c>
-      <c r="K36" t="n">
-        <v>-168.23567</v>
-      </c>
       <c r="L36" t="inlineStr">
         <is>
           <t>168˚ 14.14' W</t>
@@ -28890,7 +28890,7 @@
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA36" t="n">
@@ -29471,11 +29471,11 @@
         </is>
       </c>
       <c r="J37" t="n">
+        <v>-168.23567</v>
+      </c>
+      <c r="K37" t="n">
         <v>64.66849999999999</v>
       </c>
-      <c r="K37" t="n">
-        <v>-168.23567</v>
-      </c>
       <c r="L37" t="inlineStr">
         <is>
           <t>168˚ 14.14' W</t>
@@ -29548,7 +29548,7 @@
       </c>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA37" t="n">
@@ -30121,11 +30121,11 @@
         </is>
       </c>
       <c r="J38" t="n">
+        <v>-168.23567</v>
+      </c>
+      <c r="K38" t="n">
         <v>64.66849999999999</v>
       </c>
-      <c r="K38" t="n">
-        <v>-168.23567</v>
-      </c>
       <c r="L38" t="inlineStr">
         <is>
           <t>168˚ 14.14' W</t>
@@ -30198,7 +30198,7 @@
       </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA38" t="n">
@@ -30771,11 +30771,11 @@
         </is>
       </c>
       <c r="J39" t="n">
+        <v>-169.13884</v>
+      </c>
+      <c r="K39" t="n">
         <v>64.98833500000001</v>
       </c>
-      <c r="K39" t="n">
-        <v>-169.13884</v>
-      </c>
       <c r="L39" t="inlineStr">
         <is>
           <t>169˚ 08.33' W</t>
@@ -30848,7 +30848,7 @@
       </c>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA39" t="n">
@@ -31429,11 +31429,11 @@
         </is>
       </c>
       <c r="J40" t="n">
+        <v>-169.13884</v>
+      </c>
+      <c r="K40" t="n">
         <v>64.98833500000001</v>
       </c>
-      <c r="K40" t="n">
-        <v>-169.13884</v>
-      </c>
       <c r="L40" t="inlineStr">
         <is>
           <t>169˚ 08.33' W</t>
@@ -31506,7 +31506,7 @@
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA40" t="n">
@@ -32087,11 +32087,11 @@
         </is>
       </c>
       <c r="J41" t="n">
+        <v>-169.13884</v>
+      </c>
+      <c r="K41" t="n">
         <v>64.98833500000001</v>
       </c>
-      <c r="K41" t="n">
-        <v>-169.13884</v>
-      </c>
       <c r="L41" t="inlineStr">
         <is>
           <t>169˚ 08.33' W</t>
@@ -32164,7 +32164,7 @@
       </c>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA41" t="n">
@@ -32745,11 +32745,11 @@
         </is>
       </c>
       <c r="J42" t="n">
+        <v>-169.87915</v>
+      </c>
+      <c r="K42" t="n">
         <v>64.95945</v>
       </c>
-      <c r="K42" t="n">
-        <v>-169.87915</v>
-      </c>
       <c r="L42" t="inlineStr">
         <is>
           <t>169˚ 52.749' W</t>
@@ -32822,7 +32822,7 @@
       </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA42" t="n">
@@ -33403,11 +33403,11 @@
         </is>
       </c>
       <c r="J43" t="n">
+        <v>-169.87915</v>
+      </c>
+      <c r="K43" t="n">
         <v>64.95945</v>
       </c>
-      <c r="K43" t="n">
-        <v>-169.87915</v>
-      </c>
       <c r="L43" t="inlineStr">
         <is>
           <t>169˚ 52.749' W</t>
@@ -33480,7 +33480,7 @@
       </c>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA43" t="n">
@@ -34061,11 +34061,11 @@
         </is>
       </c>
       <c r="J44" t="n">
+        <v>-169.87915</v>
+      </c>
+      <c r="K44" t="n">
         <v>64.95945</v>
       </c>
-      <c r="K44" t="n">
-        <v>-169.87915</v>
-      </c>
       <c r="L44" t="inlineStr">
         <is>
           <t>169˚ 52.749' W</t>
@@ -34138,7 +34138,7 @@
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA44" t="n">
@@ -34711,11 +34711,11 @@
         </is>
       </c>
       <c r="J45" t="n">
+        <v>-169.87915</v>
+      </c>
+      <c r="K45" t="n">
         <v>64.95945</v>
       </c>
-      <c r="K45" t="n">
-        <v>-169.87915</v>
-      </c>
       <c r="L45" t="inlineStr">
         <is>
           <t>169˚ 52.749' W</t>
@@ -34788,7 +34788,7 @@
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA45" t="n">
@@ -35361,11 +35361,11 @@
         </is>
       </c>
       <c r="J46" t="n">
+        <v>-168.9421</v>
+      </c>
+      <c r="K46" t="n">
         <v>67.6729</v>
       </c>
-      <c r="K46" t="n">
-        <v>-168.9421</v>
-      </c>
       <c r="L46" t="inlineStr">
         <is>
           <t>168˚ 56.526' W</t>
@@ -35438,7 +35438,7 @@
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA46" t="n">
@@ -36019,11 +36019,11 @@
         </is>
       </c>
       <c r="J47" t="n">
+        <v>-168.9421</v>
+      </c>
+      <c r="K47" t="n">
         <v>67.6729</v>
       </c>
-      <c r="K47" t="n">
-        <v>-168.9421</v>
-      </c>
       <c r="L47" t="inlineStr">
         <is>
           <t>168˚ 56.526' W</t>
@@ -36096,7 +36096,7 @@
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA47" t="n">
@@ -36673,15 +36673,15 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>E49.1B.DY2012 | E49.2B.DY2012</t>
+          <t>E49.2B.DY2012 | E49.1B.DY2012</t>
         </is>
       </c>
       <c r="J48" t="n">
+        <v>-168.9421</v>
+      </c>
+      <c r="K48" t="n">
         <v>67.6729</v>
       </c>
-      <c r="K48" t="n">
-        <v>-168.9421</v>
-      </c>
       <c r="L48" t="inlineStr">
         <is>
           <t>168˚ 56.526' W</t>
@@ -36754,7 +36754,7 @@
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA48" t="n">
@@ -37331,15 +37331,15 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>E49.1B.DY2012 | E49.2B.DY2012</t>
+          <t>E49.2B.DY2012 | E49.1B.DY2012</t>
         </is>
       </c>
       <c r="J49" t="n">
+        <v>-168.9421</v>
+      </c>
+      <c r="K49" t="n">
         <v>67.6729</v>
       </c>
-      <c r="K49" t="n">
-        <v>-168.9421</v>
-      </c>
       <c r="L49" t="inlineStr">
         <is>
           <t>168˚ 56.526' W</t>
@@ -37412,7 +37412,7 @@
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA49" t="n">
@@ -37993,11 +37993,11 @@
         </is>
       </c>
       <c r="J50" t="n">
+        <v>-168.2315</v>
+      </c>
+      <c r="K50" t="n">
         <v>67.89767000000001</v>
       </c>
-      <c r="K50" t="n">
-        <v>-168.2315</v>
-      </c>
       <c r="L50" t="inlineStr">
         <is>
           <t>168˚ 13.89' W</t>
@@ -38070,7 +38070,7 @@
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA50" t="n">
@@ -38651,11 +38651,11 @@
         </is>
       </c>
       <c r="J51" t="n">
+        <v>-168.2315</v>
+      </c>
+      <c r="K51" t="n">
         <v>67.89767000000001</v>
       </c>
-      <c r="K51" t="n">
-        <v>-168.2315</v>
-      </c>
       <c r="L51" t="inlineStr">
         <is>
           <t>168˚ 13.89' W</t>
@@ -38728,7 +38728,7 @@
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA51" t="n">
@@ -39309,11 +39309,11 @@
         </is>
       </c>
       <c r="J52" t="n">
+        <v>-168.2315</v>
+      </c>
+      <c r="K52" t="n">
         <v>67.89767000000001</v>
       </c>
-      <c r="K52" t="n">
-        <v>-168.2315</v>
-      </c>
       <c r="L52" t="inlineStr">
         <is>
           <t>168˚ 13.89' W</t>
@@ -39386,7 +39386,7 @@
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA52" t="n">
@@ -39967,11 +39967,11 @@
         </is>
       </c>
       <c r="J53" t="n">
+        <v>-168.2315</v>
+      </c>
+      <c r="K53" t="n">
         <v>67.89767000000001</v>
       </c>
-      <c r="K53" t="n">
-        <v>-168.2315</v>
-      </c>
       <c r="L53" t="inlineStr">
         <is>
           <t>168˚ 13.89' W</t>
@@ -40044,7 +40044,7 @@
       </c>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA53" t="n">
@@ -40625,11 +40625,11 @@
         </is>
       </c>
       <c r="J54" t="n">
+        <v>-167.28984</v>
+      </c>
+      <c r="K54" t="n">
         <v>68.187</v>
       </c>
-      <c r="K54" t="n">
-        <v>-167.28984</v>
-      </c>
       <c r="L54" t="inlineStr">
         <is>
           <t>167˚ 17.39' W</t>
@@ -40702,7 +40702,7 @@
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA54" t="n">
@@ -41283,11 +41283,11 @@
         </is>
       </c>
       <c r="J55" t="n">
+        <v>-167.28984</v>
+      </c>
+      <c r="K55" t="n">
         <v>68.187</v>
       </c>
-      <c r="K55" t="n">
-        <v>-167.28984</v>
-      </c>
       <c r="L55" t="inlineStr">
         <is>
           <t>167˚ 17.39' W</t>
@@ -41360,7 +41360,7 @@
       </c>
       <c r="Z55" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA55" t="n">
@@ -41937,15 +41937,15 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>E53.2B.DY2012 | E53.1B.DY2012</t>
+          <t>E53.1B.DY2012 | E53.2B.DY2012</t>
         </is>
       </c>
       <c r="J56" t="n">
+        <v>-167.28984</v>
+      </c>
+      <c r="K56" t="n">
         <v>68.187</v>
       </c>
-      <c r="K56" t="n">
-        <v>-167.28984</v>
-      </c>
       <c r="L56" t="inlineStr">
         <is>
           <t>167˚ 17.39' W</t>
@@ -42018,7 +42018,7 @@
       </c>
       <c r="Z56" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA56" t="n">
@@ -42587,15 +42587,15 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>E53.2B.DY2012 | E53.1B.DY2012</t>
+          <t>E53.1B.DY2012 | E53.2B.DY2012</t>
         </is>
       </c>
       <c r="J57" t="n">
+        <v>-167.28984</v>
+      </c>
+      <c r="K57" t="n">
         <v>68.187</v>
       </c>
-      <c r="K57" t="n">
-        <v>-167.28984</v>
-      </c>
       <c r="L57" t="inlineStr">
         <is>
           <t>167˚ 17.39' W</t>
@@ -42668,7 +42668,7 @@
       </c>
       <c r="Z57" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA57" t="n">
@@ -43237,15 +43237,15 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>E54.2B.DY2012 | E54.1B.DY2012</t>
+          <t>E54.1B.DY2012 | E54.2B.DY2012</t>
         </is>
       </c>
       <c r="J58" t="n">
+        <v>-166.92484</v>
+      </c>
+      <c r="K58" t="n">
         <v>68.303</v>
       </c>
-      <c r="K58" t="n">
-        <v>-166.92484</v>
-      </c>
       <c r="L58" t="inlineStr">
         <is>
           <t>166˚ 55.49' W</t>
@@ -43318,7 +43318,7 @@
       </c>
       <c r="Z58" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA58" t="n">
@@ -43895,15 +43895,15 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>E54.2B.DY2012 | E54.1B.DY2012</t>
+          <t>E54.1B.DY2012 | E54.2B.DY2012</t>
         </is>
       </c>
       <c r="J59" t="n">
+        <v>-166.92484</v>
+      </c>
+      <c r="K59" t="n">
         <v>68.303</v>
       </c>
-      <c r="K59" t="n">
-        <v>-166.92484</v>
-      </c>
       <c r="L59" t="inlineStr">
         <is>
           <t>166˚ 55.49' W</t>
@@ -43976,7 +43976,7 @@
       </c>
       <c r="Z59" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA59" t="n">
@@ -44557,11 +44557,11 @@
         </is>
       </c>
       <c r="J60" t="n">
+        <v>-166.92484</v>
+      </c>
+      <c r="K60" t="n">
         <v>68.303</v>
       </c>
-      <c r="K60" t="n">
-        <v>-166.92484</v>
-      </c>
       <c r="L60" t="inlineStr">
         <is>
           <t>166˚ 55.49' W</t>
@@ -44634,7 +44634,7 @@
       </c>
       <c r="Z60" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA60" t="n">
@@ -45215,11 +45215,11 @@
         </is>
       </c>
       <c r="J61" t="n">
+        <v>-166.92484</v>
+      </c>
+      <c r="K61" t="n">
         <v>68.303</v>
       </c>
-      <c r="K61" t="n">
-        <v>-166.92484</v>
-      </c>
       <c r="L61" t="inlineStr">
         <is>
           <t>166˚ 55.49' W</t>
@@ -45292,7 +45292,7 @@
       </c>
       <c r="Z61" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA61" t="n">
@@ -45869,15 +45869,15 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>E57.1B.DY2012 | E57.2B.DY2012</t>
+          <t>E57.2B.DY2012 | E57.1B.DY2012</t>
         </is>
       </c>
       <c r="J62" t="n">
+        <v>-165.58417</v>
+      </c>
+      <c r="K62" t="n">
         <v>71.70517</v>
       </c>
-      <c r="K62" t="n">
-        <v>-165.58417</v>
-      </c>
       <c r="L62" t="inlineStr">
         <is>
           <t>165˚ 35.05' W</t>
@@ -45950,7 +45950,7 @@
       </c>
       <c r="Z62" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA62" t="n">
@@ -46527,15 +46527,15 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>E57.1B.DY2012 | E57.2B.DY2012</t>
+          <t>E57.2B.DY2012 | E57.1B.DY2012</t>
         </is>
       </c>
       <c r="J63" t="n">
+        <v>-165.58417</v>
+      </c>
+      <c r="K63" t="n">
         <v>71.70517</v>
       </c>
-      <c r="K63" t="n">
-        <v>-165.58417</v>
-      </c>
       <c r="L63" t="inlineStr">
         <is>
           <t>165˚ 35.05' W</t>
@@ -46608,7 +46608,7 @@
       </c>
       <c r="Z63" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA63" t="n">
@@ -47189,11 +47189,11 @@
         </is>
       </c>
       <c r="J64" t="n">
+        <v>-165.58417</v>
+      </c>
+      <c r="K64" t="n">
         <v>71.70517</v>
       </c>
-      <c r="K64" t="n">
-        <v>-165.58417</v>
-      </c>
       <c r="L64" t="inlineStr">
         <is>
           <t>165˚ 35.05' W</t>
@@ -47266,7 +47266,7 @@
       </c>
       <c r="Z64" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA64" t="n">
@@ -47839,11 +47839,11 @@
         </is>
       </c>
       <c r="J65" t="n">
+        <v>-165.58417</v>
+      </c>
+      <c r="K65" t="n">
         <v>71.70517</v>
       </c>
-      <c r="K65" t="n">
-        <v>-165.58417</v>
-      </c>
       <c r="L65" t="inlineStr">
         <is>
           <t>165˚ 35.05' W</t>
@@ -47916,7 +47916,7 @@
       </c>
       <c r="Z65" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA65" t="n">
@@ -48485,15 +48485,15 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>E59.1B.DY2012 | E59.2B.DY2012</t>
+          <t>E59.2B.DY2012 | E59.1B.DY2012</t>
         </is>
       </c>
       <c r="J66" t="n">
+        <v>-161.7726</v>
+      </c>
+      <c r="K66" t="n">
         <v>71.72410000000001</v>
       </c>
-      <c r="K66" t="n">
-        <v>-161.7726</v>
-      </c>
       <c r="L66" t="inlineStr">
         <is>
           <t>161˚ 46.356' W</t>
@@ -48566,7 +48566,7 @@
       </c>
       <c r="Z66" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA66" t="n">
@@ -49143,15 +49143,15 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>E59.1B.DY2012 | E59.2B.DY2012</t>
+          <t>E59.2B.DY2012 | E59.1B.DY2012</t>
         </is>
       </c>
       <c r="J67" t="n">
+        <v>-161.7726</v>
+      </c>
+      <c r="K67" t="n">
         <v>71.72410000000001</v>
       </c>
-      <c r="K67" t="n">
-        <v>-161.7726</v>
-      </c>
       <c r="L67" t="inlineStr">
         <is>
           <t>161˚ 46.356' W</t>
@@ -49224,7 +49224,7 @@
       </c>
       <c r="Z67" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA67" t="n">
@@ -49805,11 +49805,11 @@
         </is>
       </c>
       <c r="J68" t="n">
+        <v>-161.7726</v>
+      </c>
+      <c r="K68" t="n">
         <v>71.72410000000001</v>
       </c>
-      <c r="K68" t="n">
-        <v>-161.7726</v>
-      </c>
       <c r="L68" t="inlineStr">
         <is>
           <t>161˚ 46.356' W</t>
@@ -49882,7 +49882,7 @@
       </c>
       <c r="Z68" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA68" t="n">
@@ -50463,11 +50463,11 @@
         </is>
       </c>
       <c r="J69" t="n">
+        <v>-161.7726</v>
+      </c>
+      <c r="K69" t="n">
         <v>71.72410000000001</v>
       </c>
-      <c r="K69" t="n">
-        <v>-161.7726</v>
-      </c>
       <c r="L69" t="inlineStr">
         <is>
           <t>161˚ 46.356' W</t>
@@ -50540,7 +50540,7 @@
       </c>
       <c r="Z69" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA69" t="n">
@@ -51121,11 +51121,11 @@
         </is>
       </c>
       <c r="J70" t="n">
+        <v>-161.0373</v>
+      </c>
+      <c r="K70" t="n">
         <v>71.45489999999999</v>
       </c>
-      <c r="K70" t="n">
-        <v>-161.0373</v>
-      </c>
       <c r="L70" t="inlineStr">
         <is>
           <t>161˚ 02.238' W</t>
@@ -51198,7 +51198,7 @@
       </c>
       <c r="Z70" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA70" t="n">
@@ -51779,11 +51779,11 @@
         </is>
       </c>
       <c r="J71" t="n">
+        <v>-161.0373</v>
+      </c>
+      <c r="K71" t="n">
         <v>71.45489999999999</v>
       </c>
-      <c r="K71" t="n">
-        <v>-161.0373</v>
-      </c>
       <c r="L71" t="inlineStr">
         <is>
           <t>161˚ 02.238' W</t>
@@ -51856,7 +51856,7 @@
       </c>
       <c r="Z71" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA71" t="n">
@@ -52437,11 +52437,11 @@
         </is>
       </c>
       <c r="J72" t="n">
+        <v>-161.0373</v>
+      </c>
+      <c r="K72" t="n">
         <v>71.45489999999999</v>
       </c>
-      <c r="K72" t="n">
-        <v>-161.0373</v>
-      </c>
       <c r="L72" t="inlineStr">
         <is>
           <t>161˚ 02.238' W</t>
@@ -52514,7 +52514,7 @@
       </c>
       <c r="Z72" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA72" t="n">
@@ -53087,11 +53087,11 @@
         </is>
       </c>
       <c r="J73" t="n">
+        <v>-161.0373</v>
+      </c>
+      <c r="K73" t="n">
         <v>71.45489999999999</v>
       </c>
-      <c r="K73" t="n">
-        <v>-161.0373</v>
-      </c>
       <c r="L73" t="inlineStr">
         <is>
           <t>161˚ 02.238' W</t>
@@ -53164,7 +53164,7 @@
       </c>
       <c r="Z73" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA73" t="n">
@@ -53733,15 +53733,15 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>E63.2B.DY2012 | E63.1B.DY2012</t>
+          <t>E63.1B.DY2012 | E63.2B.DY2012</t>
         </is>
       </c>
       <c r="J74" t="n">
+        <v>-160.192</v>
+      </c>
+      <c r="K74" t="n">
         <v>71.19283</v>
       </c>
-      <c r="K74" t="n">
-        <v>-160.192</v>
-      </c>
       <c r="L74" t="inlineStr">
         <is>
           <t>160˚ 16.52' W</t>
@@ -53814,7 +53814,7 @@
       </c>
       <c r="Z74" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA74" t="n">
@@ -54391,15 +54391,15 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>E63.2B.DY2012 | E63.1B.DY2012</t>
+          <t>E63.1B.DY2012 | E63.2B.DY2012</t>
         </is>
       </c>
       <c r="J75" t="n">
+        <v>-160.192</v>
+      </c>
+      <c r="K75" t="n">
         <v>71.19283</v>
       </c>
-      <c r="K75" t="n">
-        <v>-160.192</v>
-      </c>
       <c r="L75" t="inlineStr">
         <is>
           <t>160˚ 16.52' W</t>
@@ -54472,7 +54472,7 @@
       </c>
       <c r="Z75" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA75" t="n">
@@ -55053,11 +55053,11 @@
         </is>
       </c>
       <c r="J76" t="n">
+        <v>-160.192</v>
+      </c>
+      <c r="K76" t="n">
         <v>71.19283</v>
       </c>
-      <c r="K76" t="n">
-        <v>-160.192</v>
-      </c>
       <c r="L76" t="inlineStr">
         <is>
           <t>160˚ 16.52' W</t>
@@ -55130,7 +55130,7 @@
       </c>
       <c r="Z76" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA76" t="n">
@@ -55703,11 +55703,11 @@
         </is>
       </c>
       <c r="J77" t="n">
+        <v>-160.192</v>
+      </c>
+      <c r="K77" t="n">
         <v>71.19283</v>
       </c>
-      <c r="K77" t="n">
-        <v>-160.192</v>
-      </c>
       <c r="L77" t="inlineStr">
         <is>
           <t>160˚ 16.52' W</t>
@@ -55780,7 +55780,7 @@
       </c>
       <c r="Z77" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA77" t="n">
@@ -56353,11 +56353,11 @@
         </is>
       </c>
       <c r="J78" t="n">
+        <v>-157.14107</v>
+      </c>
+      <c r="K78" t="n">
         <v>71.25239999999999</v>
       </c>
-      <c r="K78" t="n">
-        <v>-157.14107</v>
-      </c>
       <c r="L78" t="inlineStr">
         <is>
           <t>157˚ 08.464' W</t>
@@ -56430,7 +56430,7 @@
       </c>
       <c r="Z78" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA78" t="n">
@@ -57011,11 +57011,11 @@
         </is>
       </c>
       <c r="J79" t="n">
+        <v>-157.14107</v>
+      </c>
+      <c r="K79" t="n">
         <v>71.25239999999999</v>
       </c>
-      <c r="K79" t="n">
-        <v>-157.14107</v>
-      </c>
       <c r="L79" t="inlineStr">
         <is>
           <t>157˚ 08.464' W</t>
@@ -57088,7 +57088,7 @@
       </c>
       <c r="Z79" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA79" t="n">
@@ -57669,11 +57669,11 @@
         </is>
       </c>
       <c r="J80" t="n">
+        <v>-157.14107</v>
+      </c>
+      <c r="K80" t="n">
         <v>71.25239999999999</v>
       </c>
-      <c r="K80" t="n">
-        <v>-157.14107</v>
-      </c>
       <c r="L80" t="inlineStr">
         <is>
           <t>157˚ 08.464' W</t>
@@ -57746,7 +57746,7 @@
       </c>
       <c r="Z80" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA80" t="n">
@@ -58319,11 +58319,11 @@
         </is>
       </c>
       <c r="J81" t="n">
+        <v>-157.14107</v>
+      </c>
+      <c r="K81" t="n">
         <v>71.25239999999999</v>
       </c>
-      <c r="K81" t="n">
-        <v>-157.14107</v>
-      </c>
       <c r="L81" t="inlineStr">
         <is>
           <t>157˚ 08.464' W</t>
@@ -58396,7 +58396,7 @@
       </c>
       <c r="Z81" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA81" t="n">
@@ -58969,11 +58969,11 @@
         </is>
       </c>
       <c r="J82" t="n">
+        <v>-157.47517</v>
+      </c>
+      <c r="K82" t="n">
         <v>71.40667000000001</v>
       </c>
-      <c r="K82" t="n">
-        <v>-157.47517</v>
-      </c>
       <c r="L82" t="inlineStr">
         <is>
           <t>157˚ 28.51' W</t>
@@ -59046,7 +59046,7 @@
       </c>
       <c r="Z82" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA82" t="n">
@@ -59627,11 +59627,11 @@
         </is>
       </c>
       <c r="J83" t="n">
+        <v>-157.47517</v>
+      </c>
+      <c r="K83" t="n">
         <v>71.40667000000001</v>
       </c>
-      <c r="K83" t="n">
-        <v>-157.47517</v>
-      </c>
       <c r="L83" t="inlineStr">
         <is>
           <t>157˚ 28.51' W</t>
@@ -59704,7 +59704,7 @@
       </c>
       <c r="Z83" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA83" t="n">
@@ -60285,11 +60285,11 @@
         </is>
       </c>
       <c r="J84" t="n">
+        <v>-157.47517</v>
+      </c>
+      <c r="K84" t="n">
         <v>71.40667000000001</v>
       </c>
-      <c r="K84" t="n">
-        <v>-157.47517</v>
-      </c>
       <c r="L84" t="inlineStr">
         <is>
           <t>157˚ 28.51' W</t>
@@ -60362,7 +60362,7 @@
       </c>
       <c r="Z84" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA84" t="n">
@@ -60943,11 +60943,11 @@
         </is>
       </c>
       <c r="J85" t="n">
+        <v>-157.47517</v>
+      </c>
+      <c r="K85" t="n">
         <v>71.40667000000001</v>
       </c>
-      <c r="K85" t="n">
-        <v>-157.47517</v>
-      </c>
       <c r="L85" t="inlineStr">
         <is>
           <t>157˚ 28.51' W</t>
@@ -61020,7 +61020,7 @@
       </c>
       <c r="Z85" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA85" t="n">
@@ -61597,15 +61597,15 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>E69.2B.DY2012 | E69.1B.DY2012</t>
+          <t>E69.1B.DY2012 | E69.2B.DY2012</t>
         </is>
       </c>
       <c r="J86" t="n">
+        <v>-157.80038</v>
+      </c>
+      <c r="K86" t="n">
         <v>71.58055</v>
       </c>
-      <c r="K86" t="n">
-        <v>-157.80038</v>
-      </c>
       <c r="L86" t="inlineStr">
         <is>
           <t>157˚ 48.023' W</t>
@@ -61678,7 +61678,7 @@
       </c>
       <c r="Z86" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA86" t="n">
@@ -62255,15 +62255,15 @@
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>E69.2B.DY2012 | E69.1B.DY2012</t>
+          <t>E69.1B.DY2012 | E69.2B.DY2012</t>
         </is>
       </c>
       <c r="J87" t="n">
+        <v>-157.80038</v>
+      </c>
+      <c r="K87" t="n">
         <v>71.58055</v>
       </c>
-      <c r="K87" t="n">
-        <v>-157.80038</v>
-      </c>
       <c r="L87" t="inlineStr">
         <is>
           <t>157˚ 48.023' W</t>
@@ -62336,7 +62336,7 @@
       </c>
       <c r="Z87" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA87" t="n">
@@ -62913,15 +62913,15 @@
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>E70.2B.DY2012 | E70.1B.DY2012</t>
+          <t>E70.1B.DY2012 | E70.2B.DY2012</t>
         </is>
       </c>
       <c r="J88" t="n">
+        <v>-157.80038</v>
+      </c>
+      <c r="K88" t="n">
         <v>71.58055</v>
       </c>
-      <c r="K88" t="n">
-        <v>-157.80038</v>
-      </c>
       <c r="L88" t="inlineStr">
         <is>
           <t>157˚ 48.023' W</t>
@@ -62994,7 +62994,7 @@
       </c>
       <c r="Z88" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA88" t="n">
@@ -63571,15 +63571,15 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>E70.2B.DY2012 | E70.1B.DY2012</t>
+          <t>E70.1B.DY2012 | E70.2B.DY2012</t>
         </is>
       </c>
       <c r="J89" t="n">
+        <v>-157.80038</v>
+      </c>
+      <c r="K89" t="n">
         <v>71.58055</v>
       </c>
-      <c r="K89" t="n">
-        <v>-157.80038</v>
-      </c>
       <c r="L89" t="inlineStr">
         <is>
           <t>157˚ 48.023' W</t>
@@ -63652,7 +63652,7 @@
       </c>
       <c r="Z89" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA89" t="n">
@@ -64233,11 +64233,11 @@
         </is>
       </c>
       <c r="J90" t="n">
+        <v>-167.94366</v>
+      </c>
+      <c r="K90" t="n">
         <v>63.999332</v>
       </c>
-      <c r="K90" t="n">
-        <v>-167.94366</v>
-      </c>
       <c r="L90" t="inlineStr">
         <is>
           <t>167˚ 56.62' W</t>
@@ -64310,7 +64310,7 @@
       </c>
       <c r="Z90" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA90" t="n">
@@ -64891,11 +64891,11 @@
         </is>
       </c>
       <c r="J91" t="n">
+        <v>-167.94366</v>
+      </c>
+      <c r="K91" t="n">
         <v>63.999332</v>
       </c>
-      <c r="K91" t="n">
-        <v>-167.94366</v>
-      </c>
       <c r="L91" t="inlineStr">
         <is>
           <t>167˚ 56.62' W</t>
@@ -64968,7 +64968,7 @@
       </c>
       <c r="Z91" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA91" t="n">
@@ -65545,15 +65545,15 @@
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>E72.1B.DY2012 | E72.2B.DY2012</t>
+          <t>E72.2B.DY2012 | E72.1B.DY2012</t>
         </is>
       </c>
       <c r="J92" t="n">
+        <v>-167.94366</v>
+      </c>
+      <c r="K92" t="n">
         <v>63.999332</v>
       </c>
-      <c r="K92" t="n">
-        <v>-167.94366</v>
-      </c>
       <c r="L92" t="inlineStr">
         <is>
           <t>167˚ 56.62' W</t>
@@ -65626,7 +65626,7 @@
       </c>
       <c r="Z92" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA92" t="n">
@@ -66195,15 +66195,15 @@
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>E72.1B.DY2012 | E72.2B.DY2012</t>
+          <t>E72.2B.DY2012 | E72.1B.DY2012</t>
         </is>
       </c>
       <c r="J93" t="n">
+        <v>-167.94366</v>
+      </c>
+      <c r="K93" t="n">
         <v>63.999332</v>
       </c>
-      <c r="K93" t="n">
-        <v>-167.94366</v>
-      </c>
       <c r="L93" t="inlineStr">
         <is>
           <t>167˚ 56.62' W</t>
@@ -66276,7 +66276,7 @@
       </c>
       <c r="Z93" t="inlineStr">
         <is>
-          <t>CTD Niskin</t>
+          <t>Niskin Bottle</t>
         </is>
       </c>
       <c r="AA93" t="n">
@@ -67454,32 +67454,50 @@
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EB94" t="n">
-        <v/>
-      </c>
-      <c r="EC94" t="n">
-        <v/>
-      </c>
-      <c r="ED94" t="n">
-        <v/>
-      </c>
-      <c r="EE94" t="n">
-        <v/>
-      </c>
-      <c r="EF94" t="n">
-        <v/>
-      </c>
-      <c r="EG94" t="n">
-        <v/>
-      </c>
-      <c r="EH94" t="n">
-        <v/>
-      </c>
-      <c r="EI94" t="n">
-        <v/>
-      </c>
-      <c r="EJ94" t="n">
-        <v/>
+      <c r="EB94" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EC94" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="ED94" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EE94" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EF94" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EG94" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EH94" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EI94" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EJ94" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
       </c>
     </row>
     <row r="95">
@@ -68132,32 +68150,50 @@
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EB95" t="n">
-        <v/>
-      </c>
-      <c r="EC95" t="n">
-        <v/>
-      </c>
-      <c r="ED95" t="n">
-        <v/>
-      </c>
-      <c r="EE95" t="n">
-        <v/>
-      </c>
-      <c r="EF95" t="n">
-        <v/>
-      </c>
-      <c r="EG95" t="n">
-        <v/>
-      </c>
-      <c r="EH95" t="n">
-        <v/>
-      </c>
-      <c r="EI95" t="n">
-        <v/>
-      </c>
-      <c r="EJ95" t="n">
-        <v/>
+      <c r="EB95" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EC95" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="ED95" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EE95" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EF95" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EG95" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EH95" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EI95" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EJ95" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
       </c>
     </row>
     <row r="96">
@@ -68810,32 +68846,50 @@
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EB96" t="n">
-        <v/>
-      </c>
-      <c r="EC96" t="n">
-        <v/>
-      </c>
-      <c r="ED96" t="n">
-        <v/>
-      </c>
-      <c r="EE96" t="n">
-        <v/>
-      </c>
-      <c r="EF96" t="n">
-        <v/>
-      </c>
-      <c r="EG96" t="n">
-        <v/>
-      </c>
-      <c r="EH96" t="n">
-        <v/>
-      </c>
-      <c r="EI96" t="n">
-        <v/>
-      </c>
-      <c r="EJ96" t="n">
-        <v/>
+      <c r="EB96" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EC96" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="ED96" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EE96" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EF96" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EG96" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EH96" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EI96" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EJ96" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
       </c>
     </row>
     <row r="97">
@@ -69488,32 +69542,50 @@
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EB97" t="n">
-        <v/>
-      </c>
-      <c r="EC97" t="n">
-        <v/>
-      </c>
-      <c r="ED97" t="n">
-        <v/>
-      </c>
-      <c r="EE97" t="n">
-        <v/>
-      </c>
-      <c r="EF97" t="n">
-        <v/>
-      </c>
-      <c r="EG97" t="n">
-        <v/>
-      </c>
-      <c r="EH97" t="n">
-        <v/>
-      </c>
-      <c r="EI97" t="n">
-        <v/>
-      </c>
-      <c r="EJ97" t="n">
-        <v/>
+      <c r="EB97" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EC97" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="ED97" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EE97" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EF97" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EG97" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EH97" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EI97" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
+      </c>
+      <c r="EJ97" t="inlineStr">
+        <is>
+          <t>not applicable: control sample</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>